<commit_message>
final error handling+ styling
</commit_message>
<xml_diff>
--- a/misc/SCHEME_PUL.xlsx
+++ b/misc/SCHEME_PUL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotr\Documents\_TAXUS_PRACA_ZDALNA\_WDROZENIA\__ZLECENIA\PUR dla PUL\_RELEASE_PREFINAL_FILES\source\programmable+ non_ui_file\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0358A9AD-673C-4D6F-8088-AAC529C1EA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F10769-EE12-4A2D-9D1D-AB1597858D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="660" windowWidth="28800" windowHeight="15540" firstSheet="2" activeTab="5" xr2:uid="{79482166-01B3-43AE-9F51-CCA2C31AB1A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" firstSheet="25" activeTab="28" xr2:uid="{79482166-01B3-43AE-9F51-CCA2C31AB1A2}"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="92">
   <si>
     <t>Adres leśny</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Uwilgotnienie</t>
   </si>
   <si>
-    <t>Siedlisko przyrodnicze</t>
-  </si>
-  <si>
     <t>PROPONOWANE ZMIANY TYPÓW SIEDLISKOWYCH LASU</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>Stan</t>
   </si>
   <si>
-    <t>Funkcja</t>
-  </si>
-  <si>
     <t>SIEDLISKA PRZYRODNICZE</t>
   </si>
   <si>
@@ -241,15 +235,9 @@
     <t>Kod przebudowy</t>
   </si>
   <si>
-    <t>Gatunek panujący</t>
-  </si>
-  <si>
     <t>Wskazanie</t>
   </si>
   <si>
-    <t>Pow. Wskazania [ha]</t>
-  </si>
-  <si>
     <t>PRZEBUDOWA B</t>
   </si>
   <si>
@@ -332,9 +320,6 @@
   </si>
   <si>
     <t>Użytek</t>
-  </si>
-  <si>
-    <t>Wg stanu stwierdzonego w czasie taksacji na gruncie</t>
   </si>
   <si>
     <t>Powierzchnia użytku wyjściowego podanego w kol.6 po zmianach (kol.6 - kol.8)[ha]</t>
@@ -361,6 +346,16 @@
   </si>
   <si>
     <t xml:space="preserve">Pow.[ha] </t>
+  </si>
+  <si>
+    <t>Wg stanu stwierdzonego 
+w czasie taksacji na gruncie</t>
+  </si>
+  <si>
+    <t>Opis taksacyjny</t>
+  </si>
+  <si>
+    <t>TSL</t>
   </si>
 </sst>
 </file>
@@ -527,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,23 +566,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -602,10 +585,16 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +648,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="NA_ST_PS!$A$1:$D$50" spid="_x0000_s11416"/>
+                  <a14:cameraTool cellRange="NA_ST_PS!$A$1:$D$50" spid="_x0000_s11464"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -723,7 +712,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="L_ENERG_LS!$A$1:$E$50" spid="_x0000_s11417"/>
+                  <a14:cameraTool cellRange="L_ENERG_LS!$A$1:$E$50" spid="_x0000_s11465"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1630,23 +1619,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D074F9B-BB11-4868-9B42-0947EDEC84B8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1654,9 +1642,8 @@
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1670,13 +1657,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1690,9 +1674,6 @@
         <v>4</v>
       </c>
       <c r="E3" s="5">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5">
         <v>6</v>
       </c>
     </row>
@@ -1709,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBBABF6-D2BF-432B-BF99-34454F11831A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,13 +1701,12 @@
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="51" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1735,9 +1715,8 @@
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1751,16 +1730,13 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1778,9 +1754,6 @@
       </c>
       <c r="F3" s="5">
         <v>6</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1799,22 +1772,22 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -1822,7 +1795,7 @@
       <c r="E1"/>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1830,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -1888,13 +1861,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B1"/>
-    </row>
-    <row r="2" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -1924,7 +1897,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,13 +1905,13 @@
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="8.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27" style="4" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -1992,10 +1965,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D099B9-591A-4A86-A3A1-6CC49793FC59}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,24 +1976,20 @@
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2034,16 +2003,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2058,12 +2021,6 @@
       </c>
       <c r="E3" s="5">
         <v>5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2089,14 +2046,14 @@
   <cols>
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2111,10 +2068,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -2153,7 +2110,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,14 +2119,14 @@
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2178,7 +2135,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2186,16 +2143,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -2240,7 +2197,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,15 +2205,15 @@
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2265,7 +2222,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2276,16 +2233,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2301,14 +2258,12 @@
       <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>6</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2327,7 +2282,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,15 +2290,15 @@
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -2352,7 +2307,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2363,16 +2318,16 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2388,9 +2343,7 @@
       <c r="D3" s="5">
         <v>4</v>
       </c>
-      <c r="E3" s="5">
-        <v>5</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="5">
         <v>6</v>
       </c>
@@ -2984,10 +2937,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2ED8A4A-0C84-4BF5-B089-BF949F90F02C}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,15 +2949,16 @@
     <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" style="4" customWidth="1"/>
-    <col min="5" max="7" width="4.5703125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" style="4" customWidth="1"/>
     <col min="9" max="9" width="4.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3014,9 +2968,8 @@
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3024,31 +2977,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -3075,9 +3025,6 @@
       </c>
       <c r="I3" s="5">
         <v>9</v>
-      </c>
-      <c r="J3" s="5">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3109,7 +3056,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3173,7 +3120,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3246,7 +3193,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3267,19 +3214,19 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3339,7 +3286,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
@@ -3359,16 +3306,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3415,21 +3362,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3468,31 +3415,29 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D96F16-53AB-4285-803E-E7E7737434FD}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
-      <c r="E1"/>
-    </row>
-    <row r="2" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3500,16 +3445,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -3517,12 +3459,9 @@
         <v>2</v>
       </c>
       <c r="C3" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5">
         <v>5</v>
       </c>
     </row>
@@ -3542,21 +3481,21 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E73"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1"/>
@@ -3571,10 +3510,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
@@ -3939,58 +3878,48 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1A498B-7DB0-4DC7-8F77-D6FF58ADD387}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G57"/>
+      <selection activeCell="A3" sqref="A2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12" style="4" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4006,435 +3935,335 @@
       <c r="E3" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="5">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4449,10 +4278,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5215DDCD-8DE1-4E83-84DC-44B44A074147}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H61"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4462,50 +4291,40 @@
     <col min="3" max="3" width="17.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12" style="4" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4524,482 +4343,46 @@
       <c r="F3" s="5">
         <v>6</v>
       </c>
-      <c r="G3" s="5">
-        <v>7</v>
-      </c>
-      <c r="H3" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5067,10 +4450,10 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="F4" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -5130,7 +4513,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -5142,7 +4525,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -5154,7 +4537,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="11"/>
@@ -5184,7 +4567,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -5602,7 +4985,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D83"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5616,7 +4999,7 @@
   <sheetData>
     <row r="1" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5624,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -5677,7 +5060,7 @@
   <sheetData>
     <row r="1" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5724,27 +5107,27 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="8" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="8" customWidth="1"/>
     <col min="5" max="5" width="10" style="8" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5758,13 +5141,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5823,7 +5206,7 @@
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5843,10 +5226,10 @@
         <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5888,27 +5271,27 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="16" style="8" customWidth="1"/>
     <col min="6" max="6" width="10" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5918,17 +5301,17 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5970,27 +5353,27 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16" style="8" customWidth="1"/>
-    <col min="6" max="6" width="10" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="38" style="8" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5998,19 +5381,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6052,7 +5435,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6067,7 +5450,7 @@
   <sheetData>
     <row r="1" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6081,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
@@ -6120,7 +5503,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+      <selection activeCell="E35" sqref="E34:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6129,15 +5512,15 @@
     <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="8" customWidth="1"/>
     <col min="4" max="4" width="12" style="8" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="5" style="8" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6145,22 +5528,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6202,7 +5585,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6211,15 +5594,15 @@
     <col min="2" max="2" width="9.42578125" style="8" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="8" customWidth="1"/>
     <col min="4" max="4" width="12" style="8" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="31" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6227,22 +5610,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6284,22 +5667,22 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6352,7 +5735,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I8" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,67 +5745,67 @@
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="24"/>
+      <c r="J1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>93</v>
+        <v>2</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -7028,16 +6411,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -7054,13 +6437,15 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7114,17 +6499,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4902B14-8364-4F7C-A9CD-00EF49E049EF}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10" style="4" customWidth="1"/>
+    <col min="3" max="3" width="24" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7147,7 +6532,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
@@ -7186,7 +6571,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7236,23 +6621,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FBE0F-41A5-453D-B381-E0E5A130F8C5}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -7260,9 +6644,8 @@
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -7276,13 +6659,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -7297,9 +6677,6 @@
       </c>
       <c r="E3" s="5">
         <v>5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7318,17 +6695,17 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7358,7 +6735,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>